<commit_message>
improve author identification and recall
</commit_message>
<xml_diff>
--- a/example input.xlsx
+++ b/example input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\WebRoot\hsteele\mms_lookup_v9_backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E1CE7E-D364-45B8-9410-C0D2AD95E40E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCBBBED6-03A6-4A82-A8D3-31F06138A73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A7A01D49-2CA6-49F1-9BC2-FD03B27F406D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>Title</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Instructor Last Name</t>
   </si>
   <si>
-    <t>Contributor</t>
-  </si>
-  <si>
     <t>FR-0022</t>
   </si>
   <si>
@@ -138,6 +135,12 @@
   </si>
   <si>
     <t>Smith</t>
+  </si>
+  <si>
+    <t>Contributor Last</t>
+  </si>
+  <si>
+    <t>Contributor First</t>
   </si>
 </sst>
 </file>
@@ -562,22 +565,24 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
@@ -588,27 +593,27 @@
         <v>2</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="L1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>4</v>
@@ -620,24 +625,24 @@
         <v>2022</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="84" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -651,28 +656,28 @@
         <v>2021</v>
       </c>
       <c r="H3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="K3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="73.5" x14ac:dyDescent="0.45">
       <c r="A4" s="3"/>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>8</v>
@@ -684,27 +689,27 @@
         <v>2021</v>
       </c>
       <c r="H4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="K4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="84" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -718,19 +723,19 @@
         <v>2022</v>
       </c>
       <c r="H5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="K5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.45">

</xml_diff>